<commit_message>
update metrics and price data files
</commit_message>
<xml_diff>
--- a/data/avisosbtc_metrics.xlsx
+++ b/data/avisosbtc_metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="metrics_by_year" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="16">
   <si>
     <t>year</t>
   </si>
@@ -61,6 +61,9 @@
   <si>
     <t>no</t>
   </si>
+  <si>
+    <t>1mo</t>
+  </si>
 </sst>
 </file>
 
@@ -69,7 +72,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +82,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -121,12 +132,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,18 +433,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -637,6 +649,23 @@
       </c>
       <c r="E12">
         <v>98314.9609375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>2025</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>53.33</v>
+      </c>
+      <c r="D13">
+        <v>-0.60299999999999998</v>
+      </c>
+      <c r="E13">
+        <v>89605.414099999995</v>
       </c>
     </row>
   </sheetData>
@@ -646,23 +675,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="9" ySplit="16" topLeftCell="J67" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2057,7 +2089,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:12">
       <c r="A49" s="2">
         <v>44795</v>
       </c>
@@ -2086,7 +2118,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:12">
       <c r="A50" s="2">
         <v>44823</v>
       </c>
@@ -2115,7 +2147,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:12">
       <c r="A51" s="2">
         <v>44872</v>
       </c>
@@ -2144,7 +2176,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:12">
       <c r="A52" s="2">
         <v>44921</v>
       </c>
@@ -2173,7 +2205,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:12">
       <c r="A53" s="2">
         <v>45082</v>
       </c>
@@ -2202,7 +2234,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:12">
       <c r="A54" s="2">
         <v>45152</v>
       </c>
@@ -2231,7 +2263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:12">
       <c r="A55" s="2">
         <v>45404</v>
       </c>
@@ -2260,7 +2292,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:12">
       <c r="A56" s="2">
         <v>45418</v>
       </c>
@@ -2289,7 +2321,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:12">
       <c r="A57" s="2">
         <v>45460</v>
       </c>
@@ -2318,7 +2350,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:12">
       <c r="A58" s="2">
         <v>45474</v>
       </c>
@@ -2347,7 +2379,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:12">
       <c r="A59" s="2">
         <v>45502</v>
       </c>
@@ -2376,7 +2408,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:12">
       <c r="A60" s="2">
         <v>45537</v>
       </c>
@@ -2405,25 +2437,447 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="2"/>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="2"/>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="2"/>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="2"/>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="2"/>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="2"/>
+    <row r="61" spans="1:12">
+      <c r="A61" s="2">
+        <v>45712</v>
+      </c>
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <v>30</v>
+      </c>
+      <c r="E61">
+        <v>94248.3515625</v>
+      </c>
+      <c r="F61">
+        <v>2025</v>
+      </c>
+      <c r="G61">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H61">
+        <v>-4.9262797948472097E-2</v>
+      </c>
+      <c r="I61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="2">
+        <v>45719</v>
+      </c>
+      <c r="B62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>20</v>
+      </c>
+      <c r="E62">
+        <v>80601.0390625</v>
+      </c>
+      <c r="F62">
+        <v>2025</v>
+      </c>
+      <c r="G62">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H62">
+        <v>0.11171537122515</v>
+      </c>
+      <c r="I62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="2">
+        <v>45740</v>
+      </c>
+      <c r="B63" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <v>30</v>
+      </c>
+      <c r="E63">
+        <v>82334.5234375</v>
+      </c>
+      <c r="F63">
+        <v>2025</v>
+      </c>
+      <c r="G63">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H63">
+        <v>8.8309135966752939E-2</v>
+      </c>
+      <c r="I63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B64" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64">
+        <v>3</v>
+      </c>
+      <c r="D64">
+        <v>20</v>
+      </c>
+      <c r="E64">
+        <v>78214.484375</v>
+      </c>
+      <c r="F64">
+        <v>2025</v>
+      </c>
+      <c r="G64">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H64">
+        <v>0.14563708728022931</v>
+      </c>
+      <c r="I64" t="s">
+        <v>14</v>
+      </c>
+      <c r="L64" s="3"/>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="2">
+        <v>45824</v>
+      </c>
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65">
+        <v>30</v>
+      </c>
+      <c r="E65">
+        <v>100987.140625</v>
+      </c>
+      <c r="F65">
+        <v>2025</v>
+      </c>
+      <c r="G65">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H65">
+        <v>-0.11270471163020911</v>
+      </c>
+      <c r="I65" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="2">
+        <v>45894</v>
+      </c>
+      <c r="B66" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66">
+        <v>30</v>
+      </c>
+      <c r="E66">
+        <v>108236.7109375</v>
+      </c>
+      <c r="F66">
+        <v>2025</v>
+      </c>
+      <c r="G66">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H66">
+        <v>-0.17213472872211</v>
+      </c>
+      <c r="I66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="2">
+        <v>45962</v>
+      </c>
+      <c r="B67" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67">
+        <v>30</v>
+      </c>
+      <c r="E67">
+        <v>90394.3125</v>
+      </c>
+      <c r="F67">
+        <v>2025</v>
+      </c>
+      <c r="G67">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H67">
+        <v>-8.3758899377657237E-3</v>
+      </c>
+      <c r="I67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="2">
+        <v>45964</v>
+      </c>
+      <c r="B68" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68">
+        <v>30</v>
+      </c>
+      <c r="E68">
+        <v>104719.640625</v>
+      </c>
+      <c r="F68">
+        <v>2025</v>
+      </c>
+      <c r="G68">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H68">
+        <v>-0.14433038990865041</v>
+      </c>
+      <c r="I68" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="2">
+        <v>45971</v>
+      </c>
+      <c r="B69" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69">
+        <v>20</v>
+      </c>
+      <c r="E69">
+        <v>94177.078125</v>
+      </c>
+      <c r="F69">
+        <v>2025</v>
+      </c>
+      <c r="G69">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H69">
+        <v>-4.8543277764809052E-2</v>
+      </c>
+      <c r="I69" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="2">
+        <v>45978</v>
+      </c>
+      <c r="B70" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+      <c r="D70">
+        <v>10</v>
+      </c>
+      <c r="E70">
+        <v>86805.0078125</v>
+      </c>
+      <c r="F70">
+        <v>2025</v>
+      </c>
+      <c r="G70">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H70">
+        <v>3.2260883566175291E-2</v>
+      </c>
+      <c r="I70" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="2">
+        <v>45985</v>
+      </c>
+      <c r="B71" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>20</v>
+      </c>
+      <c r="E71">
+        <v>90376.75</v>
+      </c>
+      <c r="F71">
+        <v>2025</v>
+      </c>
+      <c r="G71">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H71">
+        <v>3.2260883566175291E-2</v>
+      </c>
+      <c r="I71" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="2">
+        <v>45992</v>
+      </c>
+      <c r="B72" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72">
+        <v>20</v>
+      </c>
+      <c r="E72">
+        <v>88430.1328125</v>
+      </c>
+      <c r="F72">
+        <v>2025</v>
+      </c>
+      <c r="G72">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H72">
+        <v>1.364972364747352E-2</v>
+      </c>
+      <c r="I72" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="2">
+        <v>45999</v>
+      </c>
+      <c r="B73" t="s">
+        <v>13</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73">
+        <v>20</v>
+      </c>
+      <c r="E73">
+        <v>90162.91</v>
+      </c>
+      <c r="F73">
+        <v>2025</v>
+      </c>
+      <c r="G73">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H73">
+        <f>(G73-E73)/E73</f>
+        <v>-6.1832065979237913E-3</v>
+      </c>
+      <c r="I73" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="2">
+        <v>46006</v>
+      </c>
+      <c r="B74" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74">
+        <v>20</v>
+      </c>
+      <c r="E74">
+        <v>88230.77</v>
+      </c>
+      <c r="F74">
+        <v>2025</v>
+      </c>
+      <c r="G74">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H74">
+        <f t="shared" ref="H74:H75" si="0">(G74-E74)/E74</f>
+        <v>1.5580098643591009E-2</v>
+      </c>
+      <c r="I74" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="2">
+        <v>46013</v>
+      </c>
+      <c r="B75" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75">
+        <v>3</v>
+      </c>
+      <c r="D75">
+        <v>20</v>
+      </c>
+      <c r="E75">
+        <v>88577.42</v>
+      </c>
+      <c r="F75">
+        <v>2025</v>
+      </c>
+      <c r="G75">
+        <v>89605.414099999995</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="0"/>
+        <v>1.1605599937320327E-2</v>
+      </c>
+      <c r="I75" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>